<commit_message>
carb chem data and figure update
</commit_message>
<xml_diff>
--- a/Output/Statistics/Results_summary.xlsx
+++ b/Output/Statistics/Results_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Acclim_Dynamics\Output\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B10206-B177-4376-9833-95D8537CA258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79477FED-8C46-4886-922A-337E21BCB42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metabolism" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3704" uniqueCount="1447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3706" uniqueCount="1449">
   <si>
     <t>Timepoint</t>
   </si>
@@ -4570,6 +4570,50 @@
   </si>
   <si>
     <t>27.583 ± 0.106</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>M. capitata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Type III ANOVA; Surv(lifespan, status) ~ Temperature * CO2 + (1|PLUG.ID/Tank)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>P. acuta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Type III ANOVA; Surv(lifespan, status) ~ Temperature * CO2 + (1|PLUG.ID/Tank)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4827,7 +4871,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -4904,6 +4948,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4952,7 +5007,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5274,9 +5329,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5285,26 +5349,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5336,20 +5388,20 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="22" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5359,6 +5411,28 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -5775,8 +5849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5F79C1-D35C-C047-889A-12882B507491}">
   <dimension ref="B1:L90"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L39" sqref="H4:L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="15"/>
@@ -7135,8 +7209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C042A6-E1AB-2645-9C1D-0F0DDF171DC1}">
   <dimension ref="C3:F18"/>
   <sheetViews>
-    <sheetView zoomScale="143" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A6" zoomScale="143" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -7154,12 +7228,12 @@
       <c r="F3" s="103"/>
     </row>
     <row r="5" spans="3:6" ht="18">
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="157" t="s">
         <v>299</v>
       </c>
-      <c r="D5" s="158"/>
-      <c r="E5" s="158"/>
-      <c r="F5" s="158"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
+      <c r="F5" s="157"/>
     </row>
     <row r="6" spans="3:6" ht="16.2" thickBot="1">
       <c r="C6" s="104" t="s">
@@ -7238,12 +7312,12 @@
       <c r="F11" s="108"/>
     </row>
     <row r="12" spans="3:6" ht="18">
-      <c r="C12" s="156" t="s">
+      <c r="C12" s="152" t="s">
         <v>300</v>
       </c>
-      <c r="D12" s="156"/>
-      <c r="E12" s="156"/>
-      <c r="F12" s="156"/>
+      <c r="D12" s="152"/>
+      <c r="E12" s="152"/>
+      <c r="F12" s="152"/>
     </row>
     <row r="13" spans="3:6" ht="19.2" thickBot="1">
       <c r="C13" s="104" t="s">
@@ -7325,29 +7399,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E81509-5EAD-4D6C-9F34-F77156147463}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="8.796875" style="85"/>
-    <col min="2" max="2" width="21" style="85" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" style="85" customWidth="1"/>
-    <col min="4" max="4" width="18.796875" style="85" customWidth="1"/>
-    <col min="5" max="5" width="17" style="85" customWidth="1"/>
-    <col min="6" max="6" width="15.796875" style="85" customWidth="1"/>
-    <col min="7" max="7" width="16.8984375" style="85" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" style="85" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.19921875" style="85" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.09765625" style="85" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.09765625" style="85" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.796875" style="85"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18">
-      <c r="B2" s="159"/>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
-      <c r="E2" s="159"/>
-      <c r="F2" s="159"/>
-      <c r="G2" s="159"/>
+      <c r="B2" s="158"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
     </row>
     <row r="3" spans="2:7" ht="16.2" thickBot="1">
       <c r="B3" s="118" t="s">
@@ -9614,7 +9686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACEA87D1-2548-4A55-8922-8C853FE0093A}">
   <dimension ref="B3:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -12065,16 +12137,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34.950000000000003" customHeight="1" thickBot="1">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
     </row>
     <row r="2" spans="1:8" s="53" customFormat="1">
       <c r="A2" s="100" t="s">
@@ -26958,16 +27030,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34.950000000000003" customHeight="1" thickBot="1">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
     </row>
     <row r="2" spans="1:8" s="53" customFormat="1">
       <c r="A2" s="100" t="s">
@@ -31577,8 +31649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED3900D-0274-AF44-ABCA-72E49F338EC7}">
   <dimension ref="B1:R90"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="15"/>
@@ -33538,8 +33610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78875509-8FE0-E14D-9EA2-C2EA75893B22}">
   <dimension ref="B1:R90"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F4"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="15"/>
@@ -35248,76 +35320,78 @@
   <dimension ref="B1:I30"/>
   <sheetViews>
     <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D3" sqref="D3:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.796875" style="32"/>
-    <col min="2" max="2" width="25.69921875" style="32" customWidth="1"/>
-    <col min="3" max="3" width="32.19921875" style="32" customWidth="1"/>
-    <col min="4" max="4" width="24" style="32" customWidth="1"/>
+    <col min="2" max="2" width="23.3984375" style="32" customWidth="1"/>
+    <col min="3" max="3" width="5" style="32" customWidth="1"/>
+    <col min="4" max="4" width="23" style="32" customWidth="1"/>
     <col min="5" max="5" width="15.19921875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="12.296875" style="30" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="30" customWidth="1"/>
-    <col min="8" max="8" width="10.796875" style="30"/>
-    <col min="9" max="9" width="13.69921875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="11.8984375" style="30" customWidth="1"/>
+    <col min="7" max="7" width="14.796875" style="30" customWidth="1"/>
+    <col min="8" max="8" width="8.8984375" style="30" customWidth="1"/>
+    <col min="9" max="9" width="10" style="30" customWidth="1"/>
     <col min="10" max="16384" width="10.796875" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="16.05" customHeight="1">
-      <c r="B1" s="136" t="s">
+      <c r="B1" s="140" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
     </row>
     <row r="2" spans="2:9" ht="16.05" customHeight="1" thickBot="1">
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
     </row>
     <row r="3" spans="2:9" ht="27" customHeight="1">
       <c r="B3" s="70" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="72"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
+      <c r="D3" s="161" t="s">
+        <v>1447</v>
+      </c>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
     </row>
     <row r="4" spans="2:9" ht="18.600000000000001" thickBot="1">
-      <c r="B4" s="134" t="s">
+      <c r="B4" s="137" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="135"/>
+      <c r="C4" s="138"/>
       <c r="D4" s="69" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="138" t="s">
+      <c r="F4" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138" t="s">
+      <c r="G4" s="135"/>
+      <c r="H4" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="138"/>
+      <c r="I4" s="135"/>
     </row>
     <row r="5" spans="2:9" ht="15.6">
       <c r="D5" s="19" t="s">
@@ -35326,14 +35400,14 @@
       <c r="E5" s="20">
         <v>1</v>
       </c>
-      <c r="F5" s="139">
+      <c r="F5" s="133">
         <v>21.004000000000001</v>
       </c>
-      <c r="G5" s="139"/>
-      <c r="H5" s="141" t="s">
+      <c r="G5" s="133"/>
+      <c r="H5" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="141"/>
+      <c r="I5" s="134"/>
     </row>
     <row r="6" spans="2:9" ht="15.6">
       <c r="D6" s="19" t="s">
@@ -35342,14 +35416,14 @@
       <c r="E6" s="20">
         <v>1</v>
       </c>
-      <c r="F6" s="139">
+      <c r="F6" s="133">
         <v>11.489100000000001</v>
       </c>
-      <c r="G6" s="139"/>
-      <c r="H6" s="141">
+      <c r="G6" s="133"/>
+      <c r="H6" s="134">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="I6" s="141"/>
+      <c r="I6" s="134"/>
     </row>
     <row r="7" spans="2:9">
       <c r="D7" s="32" t="s">
@@ -35358,14 +35432,14 @@
       <c r="E7" s="30">
         <v>1</v>
       </c>
-      <c r="F7" s="140">
+      <c r="F7" s="139">
         <v>0.29139999999999999</v>
       </c>
-      <c r="G7" s="140"/>
-      <c r="H7" s="140">
+      <c r="G7" s="139"/>
+      <c r="H7" s="139">
         <v>0.58930000000000005</v>
       </c>
-      <c r="I7" s="140"/>
+      <c r="I7" s="139"/>
     </row>
     <row r="9" spans="2:9" ht="16.2" thickBot="1">
       <c r="B9" s="71" t="s">
@@ -35392,10 +35466,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="24" customHeight="1">
-      <c r="B10" s="132" t="s">
+      <c r="B10" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="132"/>
+      <c r="C10" s="136"/>
       <c r="D10" s="19" t="s">
         <v>49</v>
       </c>
@@ -35416,8 +35490,8 @@
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.6">
-      <c r="B11" s="133"/>
-      <c r="C11" s="133"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="160"/>
       <c r="D11" s="19" t="s">
         <v>50</v>
       </c>
@@ -35438,6 +35512,8 @@
       </c>
     </row>
     <row r="12" spans="2:9">
+      <c r="B12" s="160"/>
+      <c r="C12" s="160"/>
       <c r="D12" s="32" t="s">
         <v>51</v>
       </c>
@@ -35456,19 +35532,23 @@
       <c r="I12" s="35">
         <v>0.59</v>
       </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="160"/>
+      <c r="C13" s="160"/>
     </row>
     <row r="14" spans="2:9" ht="16.2" thickBot="1">
       <c r="E14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="138" t="s">
+      <c r="F14" s="135" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="138"/>
-      <c r="H14" s="138" t="s">
+      <c r="G14" s="135"/>
+      <c r="H14" s="135" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="138"/>
+      <c r="I14" s="135"/>
     </row>
     <row r="15" spans="2:9">
       <c r="D15" s="32" t="s">
@@ -35477,46 +35557,49 @@
       <c r="E15" s="30">
         <v>-7359.299</v>
       </c>
-      <c r="F15" s="142">
+      <c r="F15" s="132">
         <v>-5183.3040000000001</v>
       </c>
-      <c r="G15" s="142"/>
-      <c r="H15" s="142">
+      <c r="G15" s="132"/>
+      <c r="H15" s="132">
         <v>-4472.5200000000004</v>
       </c>
-      <c r="I15" s="142"/>
-    </row>
+      <c r="I15" s="132"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.6" thickBot="1"/>
     <row r="18" spans="2:9" ht="18.600000000000001">
       <c r="B18" s="70" t="s">
         <v>61</v>
       </c>
       <c r="C18" s="72"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="D18" s="161" t="s">
+        <v>1448</v>
+      </c>
+      <c r="E18" s="161"/>
+      <c r="F18" s="161"/>
+      <c r="G18" s="161"/>
+      <c r="H18" s="161"/>
+      <c r="I18" s="161"/>
     </row>
     <row r="19" spans="2:9" ht="18.600000000000001" thickBot="1">
-      <c r="B19" s="134" t="s">
+      <c r="B19" s="137" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="135"/>
+      <c r="C19" s="138"/>
       <c r="D19" s="69" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="138" t="s">
+      <c r="F19" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="138"/>
-      <c r="H19" s="138" t="s">
+      <c r="G19" s="135"/>
+      <c r="H19" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="138"/>
+      <c r="I19" s="135"/>
     </row>
     <row r="20" spans="2:9">
       <c r="D20" s="32" t="s">
@@ -35525,14 +35608,14 @@
       <c r="E20" s="30">
         <v>1</v>
       </c>
-      <c r="F20" s="140">
+      <c r="F20" s="139">
         <v>2.2172999999999998</v>
       </c>
-      <c r="G20" s="140"/>
-      <c r="H20" s="140">
+      <c r="G20" s="139"/>
+      <c r="H20" s="139">
         <v>0.13650000000000001</v>
       </c>
-      <c r="I20" s="140"/>
+      <c r="I20" s="139"/>
     </row>
     <row r="21" spans="2:9" ht="15.6">
       <c r="D21" s="19" t="s">
@@ -35541,14 +35624,14 @@
       <c r="E21" s="20">
         <v>1</v>
       </c>
-      <c r="F21" s="139">
+      <c r="F21" s="133">
         <v>40.541200000000003</v>
       </c>
-      <c r="G21" s="139"/>
-      <c r="H21" s="141" t="s">
+      <c r="G21" s="133"/>
+      <c r="H21" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="141"/>
+      <c r="I21" s="134"/>
     </row>
     <row r="22" spans="2:9" ht="15.6">
       <c r="D22" s="19" t="s">
@@ -35557,14 +35640,14 @@
       <c r="E22" s="20">
         <v>1</v>
       </c>
-      <c r="F22" s="139">
+      <c r="F22" s="133">
         <v>79.950599999999994</v>
       </c>
-      <c r="G22" s="139"/>
-      <c r="H22" s="141" t="s">
+      <c r="G22" s="133"/>
+      <c r="H22" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="141"/>
+      <c r="I22" s="134"/>
     </row>
     <row r="24" spans="2:9" ht="16.2" thickBot="1">
       <c r="B24" s="71" t="s">
@@ -35590,11 +35673,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15.6">
-      <c r="B25" s="132" t="s">
+    <row r="25" spans="2:9" ht="15.6" customHeight="1">
+      <c r="B25" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="132"/>
+      <c r="C25" s="136"/>
       <c r="D25" s="39" t="s">
         <v>49</v>
       </c>
@@ -35615,8 +35698,8 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="15.6">
-      <c r="B26" s="133"/>
-      <c r="C26" s="133"/>
+      <c r="B26" s="160"/>
+      <c r="C26" s="160"/>
       <c r="D26" s="19" t="s">
         <v>50</v>
       </c>
@@ -35637,6 +35720,8 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="15.6">
+      <c r="B27" s="160"/>
+      <c r="C27" s="160"/>
       <c r="D27" s="19" t="s">
         <v>51</v>
       </c>
@@ -35655,19 +35740,23 @@
       <c r="I27" s="21" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="160"/>
+      <c r="C28" s="160"/>
     </row>
     <row r="29" spans="2:9" ht="16.2" thickBot="1">
       <c r="E29" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="138" t="s">
+      <c r="F29" s="135" t="s">
         <v>59</v>
       </c>
-      <c r="G29" s="138"/>
-      <c r="H29" s="138" t="s">
+      <c r="G29" s="135"/>
+      <c r="H29" s="135" t="s">
         <v>60</v>
       </c>
-      <c r="I29" s="138"/>
+      <c r="I29" s="135"/>
     </row>
     <row r="30" spans="2:9">
       <c r="D30" s="32" t="s">
@@ -35676,36 +35765,17 @@
       <c r="E30" s="30">
         <v>-24130.77</v>
       </c>
-      <c r="F30" s="142" t="s">
+      <c r="F30" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="142"/>
-      <c r="H30" s="142">
+      <c r="G30" s="132"/>
+      <c r="H30" s="132">
         <v>-18100.5</v>
       </c>
-      <c r="I30" s="142"/>
+      <c r="I30" s="132"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B10:C11"/>
+  <mergeCells count="31">
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:I2"/>
     <mergeCell ref="F4:G4"/>
@@ -35716,6 +35786,27 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B10:C13"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B25:C28"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35725,8 +35816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21807EB-5189-2E47-85FD-BCB7055F6515}">
   <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -35741,50 +35832,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12">
-      <c r="B1" s="144" t="s">
+      <c r="B1" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
       <c r="G1" s="53"/>
-      <c r="H1" s="144" t="s">
+      <c r="H1" s="143" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="143"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="143"/>
     </row>
     <row r="2" spans="2:12" ht="27" customHeight="1">
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
       <c r="G2" s="53"/>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145"/>
-      <c r="J2" s="145"/>
-      <c r="K2" s="145"/>
-      <c r="L2" s="145"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
     </row>
     <row r="3" spans="2:12" ht="18" thickBot="1">
-      <c r="B3" s="143" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="H3" s="143" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143"/>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143"/>
+      <c r="B3" s="142" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="H3" s="142" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="142"/>
     </row>
     <row r="4" spans="2:12" ht="18.600000000000001" thickBot="1">
       <c r="B4" s="48" t="s">
@@ -36219,20 +36310,20 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="18" thickBot="1">
-      <c r="B20" s="143" t="s">
+      <c r="B20" s="142" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="143"/>
-      <c r="D20" s="143"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="143"/>
-      <c r="H20" s="143" t="s">
+      <c r="C20" s="142"/>
+      <c r="D20" s="142"/>
+      <c r="E20" s="142"/>
+      <c r="F20" s="142"/>
+      <c r="H20" s="142" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="143"/>
-      <c r="J20" s="143"/>
-      <c r="K20" s="143"/>
-      <c r="L20" s="143"/>
+      <c r="I20" s="142"/>
+      <c r="J20" s="142"/>
+      <c r="K20" s="142"/>
+      <c r="L20" s="142"/>
     </row>
     <row r="21" spans="2:12" ht="18.600000000000001" thickBot="1">
       <c r="B21" s="48" t="s">
@@ -36604,16 +36695,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9ABFAF6-E371-0746-B011-7242CD7A8CF9}">
-  <dimension ref="B1:E45"/>
+  <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.796875" style="47"/>
-    <col min="2" max="2" width="44" style="47" customWidth="1"/>
+    <col min="2" max="2" width="37.5" style="47" customWidth="1"/>
     <col min="3" max="3" width="10.296875" style="51" customWidth="1"/>
     <col min="4" max="4" width="10.796875" style="51"/>
     <col min="5" max="5" width="18.796875" style="51" customWidth="1"/>
@@ -36621,18 +36712,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="145" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
     </row>
     <row r="2" spans="2:5">
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
     </row>
     <row r="3" spans="2:5" ht="16.2" thickBot="1">
       <c r="B3" s="50" t="s">
@@ -36663,378 +36754,294 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="18">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="163" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="32"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="38"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="52" t="s">
+      <c r="B6" s="162" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C6" s="35">
         <v>-1.0843</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D6" s="59">
         <v>37.811</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E6" s="35">
         <v>0.28510000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="18">
-      <c r="B8" s="13" t="s">
+    <row r="7" spans="2:5" ht="18">
+      <c r="B7" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="35"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="36"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="38"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="35">
+        <v>1.2234</v>
+      </c>
+      <c r="D8" s="59">
+        <v>44.265999999999998</v>
+      </c>
+      <c r="E8" s="35">
+        <v>0.2276</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="18">
+      <c r="B9" s="163" t="s">
+        <v>8</v>
+      </c>
       <c r="C9" s="38"/>
       <c r="D9" s="60"/>
       <c r="E9" s="38"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="35">
-        <v>1.2234</v>
-      </c>
-      <c r="D10" s="59">
-        <v>44.265999999999998</v>
-      </c>
-      <c r="E10" s="35">
-        <v>0.2276</v>
+      <c r="B10" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="43">
+        <v>-3.4384999999999999</v>
+      </c>
+      <c r="D10" s="45">
+        <v>44.000999999999998</v>
+      </c>
+      <c r="E10" s="21">
+        <v>1.2999999999999999E-3</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="18">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="35"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="36"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="38"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="43">
-        <v>-3.4384999999999999</v>
-      </c>
-      <c r="D13" s="45">
-        <v>44.000999999999998</v>
-      </c>
-      <c r="E13" s="21">
-        <v>1.2999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="18">
-      <c r="B14" s="13" t="s">
+      <c r="B12" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="66">
+        <v>-4.0388000000000002</v>
+      </c>
+      <c r="D12" s="62">
+        <v>40.850999999999999</v>
+      </c>
+      <c r="E12" s="98">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="18">
+      <c r="B13" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="35"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="36"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="38"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="68"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="66">
+        <v>-3.0230000000000001</v>
+      </c>
+      <c r="D14" s="62">
+        <v>37.777000000000001</v>
+      </c>
+      <c r="E14" s="98">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="18">
+      <c r="B15" s="163" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="68"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="68"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="66">
-        <v>-4.0388000000000002</v>
-      </c>
-      <c r="D16" s="62">
-        <v>40.850999999999999</v>
-      </c>
-      <c r="E16" s="98">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="18">
-      <c r="B17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="67"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="55"/>
+      <c r="B16" s="164" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="165">
+        <v>-3.2361</v>
+      </c>
+      <c r="D16" s="166">
+        <v>45.631</v>
+      </c>
+      <c r="E16" s="167">
+        <v>2.3E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="67">
+        <v>1.8842000000000001</v>
+      </c>
+      <c r="D17" s="63">
+        <v>229.73</v>
+      </c>
+      <c r="E17" s="67">
+        <v>6.08E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="18">
+      <c r="B18" s="163" t="s">
+        <v>40</v>
+      </c>
       <c r="C18" s="68"/>
       <c r="D18" s="64"/>
       <c r="E18" s="68"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="66">
-        <v>-3.0230000000000001</v>
-      </c>
-      <c r="D19" s="62">
-        <v>37.777000000000001</v>
-      </c>
-      <c r="E19" s="98">
-        <v>4.4999999999999997E-3</v>
+      <c r="B19" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="67">
+        <v>0.45760000000000001</v>
+      </c>
+      <c r="D19" s="63">
+        <v>33.716999999999999</v>
+      </c>
+      <c r="E19" s="67">
+        <v>0.6502</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="18">
-      <c r="B20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="67"/>
+      <c r="B20" s="163" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="68"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="68"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="55"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="68"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="58" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="66">
-        <v>-3.2361</v>
-      </c>
-      <c r="D22" s="62">
-        <v>45.631</v>
-      </c>
-      <c r="E22" s="98">
-        <v>2.3E-3</v>
-      </c>
+      <c r="B21" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="67">
+        <v>-0.12515999999999999</v>
+      </c>
+      <c r="D21" s="63">
+        <v>37.548999999999999</v>
+      </c>
+      <c r="E21" s="67">
+        <v>0.90110000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="18">
+      <c r="B22" s="163" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="68"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="68"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="13"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="67"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="55"/>
+      <c r="B23" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="67">
+        <v>1.2561</v>
+      </c>
+      <c r="D23" s="63">
+        <v>36.850999999999999</v>
+      </c>
+      <c r="E23" s="67">
+        <v>0.217</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="18">
+      <c r="B24" s="163" t="s">
+        <v>31</v>
+      </c>
       <c r="C24" s="68"/>
       <c r="D24" s="64"/>
       <c r="E24" s="68"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="67">
-        <v>1.8842000000000001</v>
-      </c>
-      <c r="D25" s="63">
-        <v>229.73</v>
-      </c>
-      <c r="E25" s="67">
-        <v>6.08E-2</v>
+      <c r="B25" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="66">
+        <v>2.5909</v>
+      </c>
+      <c r="D25" s="62">
+        <v>30.641999999999999</v>
+      </c>
+      <c r="E25" s="98">
+        <v>1.4500000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="18">
-      <c r="B26" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="67"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="67"/>
+      <c r="B26" s="163" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="68"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="68"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="55"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="68"/>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="67">
-        <v>0.45760000000000001</v>
-      </c>
-      <c r="D28" s="63">
-        <v>33.716999999999999</v>
-      </c>
-      <c r="E28" s="67">
-        <v>0.6502</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="18">
-      <c r="B29" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="67"/>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="55"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="68"/>
+      <c r="B27" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="66">
+        <v>2.8515000000000001</v>
+      </c>
+      <c r="D27" s="62">
+        <v>28.989000000000001</v>
+      </c>
+      <c r="E27" s="98">
+        <v>7.9399999999999991E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="18">
+      <c r="B28" s="163" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="68"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="68"/>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="164" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="165">
+        <v>5.0693999999999999</v>
+      </c>
+      <c r="D29" s="166">
+        <v>34.066000000000003</v>
+      </c>
+      <c r="E29" s="167" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="67">
-        <v>-0.12515999999999999</v>
-      </c>
-      <c r="D31" s="63">
-        <v>37.548999999999999</v>
-      </c>
-      <c r="E31" s="67">
-        <v>0.90110000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="18">
-      <c r="B32" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="67"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="67"/>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="55"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="68"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="67">
-        <v>1.2561</v>
-      </c>
-      <c r="D34" s="63">
-        <v>36.850999999999999</v>
-      </c>
-      <c r="E34" s="67">
-        <v>0.217</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="18">
-      <c r="B35" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="67"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="67"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="55"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="68"/>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="66">
-        <v>2.5909</v>
-      </c>
-      <c r="D37" s="62">
-        <v>30.641999999999999</v>
-      </c>
-      <c r="E37" s="98">
-        <v>1.4500000000000001E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="18">
-      <c r="B38" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="67"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="67"/>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="55"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="68"/>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="66">
-        <v>2.8515000000000001</v>
-      </c>
-      <c r="D40" s="62">
-        <v>28.989000000000001</v>
-      </c>
-      <c r="E40" s="98">
-        <v>7.9399999999999991E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="18">
-      <c r="B41" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="67"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="67"/>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="55"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="68"/>
-    </row>
-    <row r="43" spans="2:5">
-      <c r="B43" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="66">
-        <v>5.0693999999999999</v>
-      </c>
-      <c r="D43" s="62">
-        <v>34.066000000000003</v>
-      </c>
-      <c r="E43" s="98" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="B44" s="13"/>
-      <c r="C44" s="67"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="56"/>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="B45" s="55"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="57"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="56"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="55"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -37048,56 +37055,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C362F6-C5EC-A24E-B27B-16669A93CA5C}">
   <dimension ref="B1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.796875" style="47"/>
-    <col min="2" max="2" width="42.69921875" style="85" customWidth="1"/>
-    <col min="3" max="5" width="16.5" style="51" customWidth="1"/>
-    <col min="6" max="6" width="18.19921875" style="51" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="51" customWidth="1"/>
+    <col min="2" max="2" width="38.296875" style="85" customWidth="1"/>
+    <col min="3" max="3" width="5.3984375" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="51" customWidth="1"/>
+    <col min="5" max="6" width="8.796875" style="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" style="51" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="16.5" style="47" customWidth="1"/>
     <col min="12" max="16384" width="10.796875" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="16.05" customHeight="1">
-      <c r="B1" s="149" t="s">
+      <c r="B1" s="148" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
       <c r="H1" s="81"/>
       <c r="I1" s="81"/>
       <c r="J1" s="81"/>
       <c r="K1" s="81"/>
     </row>
     <row r="2" spans="2:11" ht="22.05" customHeight="1">
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
       <c r="H2" s="81"/>
       <c r="I2" s="81"/>
       <c r="J2" s="81"/>
       <c r="K2" s="81"/>
     </row>
     <row r="3" spans="2:11" ht="25.05" customHeight="1">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="150" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="151"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
       <c r="J3" s="32"/>
@@ -37488,14 +37496,14 @@
       <c r="K19" s="32"/>
     </row>
     <row r="21" spans="2:11" ht="22.95" customHeight="1">
-      <c r="B21" s="148" t="s">
+      <c r="B21" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
+      <c r="C21" s="147"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="147"/>
+      <c r="F21" s="147"/>
+      <c r="G21" s="147"/>
     </row>
     <row r="22" spans="2:11" ht="16.2" thickBot="1">
       <c r="B22" s="84" t="s">
@@ -37666,14 +37674,14 @@
       <c r="G30" s="88"/>
     </row>
     <row r="31" spans="2:11" ht="25.95" customHeight="1">
-      <c r="B31" s="148" t="s">
+      <c r="B31" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="148"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="148"/>
-      <c r="F31" s="148"/>
-      <c r="G31" s="148"/>
+      <c r="C31" s="147"/>
+      <c r="D31" s="147"/>
+      <c r="E31" s="147"/>
+      <c r="F31" s="147"/>
+      <c r="G31" s="147"/>
     </row>
     <row r="32" spans="2:11" ht="16.2" thickBot="1">
       <c r="B32" s="84" t="s">
@@ -37836,32 +37844,32 @@
       </c>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="149" t="s">
+      <c r="B42" s="148" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="149"/>
-      <c r="D42" s="149"/>
-      <c r="E42" s="149"/>
-      <c r="F42" s="149"/>
-      <c r="G42" s="149"/>
+      <c r="C42" s="148"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="148"/>
+      <c r="F42" s="148"/>
+      <c r="G42" s="148"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="150"/>
-      <c r="C43" s="150"/>
-      <c r="D43" s="150"/>
-      <c r="E43" s="150"/>
-      <c r="F43" s="150"/>
-      <c r="G43" s="150"/>
+      <c r="B43" s="149"/>
+      <c r="C43" s="149"/>
+      <c r="D43" s="149"/>
+      <c r="E43" s="149"/>
+      <c r="F43" s="149"/>
+      <c r="G43" s="149"/>
     </row>
     <row r="44" spans="2:7" ht="25.95" customHeight="1">
-      <c r="B44" s="148" t="s">
+      <c r="B44" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="148"/>
-      <c r="D44" s="148"/>
-      <c r="E44" s="148"/>
-      <c r="F44" s="148"/>
-      <c r="G44" s="148"/>
+      <c r="C44" s="147"/>
+      <c r="D44" s="147"/>
+      <c r="E44" s="147"/>
+      <c r="F44" s="147"/>
+      <c r="G44" s="147"/>
     </row>
     <row r="45" spans="2:7" ht="16.2" thickBot="1">
       <c r="B45" s="84" t="s">
@@ -38040,56 +38048,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FF8875-836F-5542-A93E-7F77BBB5F49C}">
   <dimension ref="B1:K52"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.796875" style="47"/>
-    <col min="2" max="2" width="42.69921875" style="85" customWidth="1"/>
-    <col min="3" max="5" width="16.5" style="51" customWidth="1"/>
-    <col min="6" max="6" width="18.19921875" style="51" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="51" customWidth="1"/>
+    <col min="2" max="2" width="37.296875" style="85" customWidth="1"/>
+    <col min="3" max="3" width="5.3984375" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="51" customWidth="1"/>
+    <col min="5" max="5" width="8.296875" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.09765625" style="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" style="51" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="16.5" style="47" customWidth="1"/>
     <col min="12" max="16384" width="10.796875" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="16.05" customHeight="1">
-      <c r="B1" s="149" t="s">
+      <c r="B1" s="148" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
       <c r="H1" s="81"/>
       <c r="I1" s="81"/>
       <c r="J1" s="81"/>
       <c r="K1" s="81"/>
     </row>
     <row r="2" spans="2:11" ht="22.05" customHeight="1">
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
       <c r="H2" s="81"/>
       <c r="I2" s="81"/>
       <c r="J2" s="81"/>
       <c r="K2" s="81"/>
     </row>
     <row r="3" spans="2:11" ht="25.05" customHeight="1">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="150" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="151"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
       <c r="J3" s="32"/>
@@ -38480,14 +38490,14 @@
       <c r="K19" s="32"/>
     </row>
     <row r="21" spans="2:11" ht="22.95" customHeight="1">
-      <c r="B21" s="148" t="s">
+      <c r="B21" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
+      <c r="C21" s="147"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="147"/>
+      <c r="F21" s="147"/>
+      <c r="G21" s="147"/>
     </row>
     <row r="22" spans="2:11" ht="16.2" thickBot="1">
       <c r="B22" s="84" t="s">
@@ -38658,14 +38668,14 @@
       <c r="G30" s="88"/>
     </row>
     <row r="31" spans="2:11" ht="25.95" customHeight="1">
-      <c r="B31" s="148" t="s">
+      <c r="B31" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="148"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="148"/>
-      <c r="F31" s="148"/>
-      <c r="G31" s="148"/>
+      <c r="C31" s="147"/>
+      <c r="D31" s="147"/>
+      <c r="E31" s="147"/>
+      <c r="F31" s="147"/>
+      <c r="G31" s="147"/>
     </row>
     <row r="32" spans="2:11" ht="16.2" thickBot="1">
       <c r="B32" s="84" t="s">
@@ -38828,28 +38838,28 @@
       </c>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="149"/>
-      <c r="C42" s="149"/>
-      <c r="D42" s="149"/>
-      <c r="E42" s="149"/>
-      <c r="F42" s="149"/>
-      <c r="G42" s="149"/>
+      <c r="B42" s="148"/>
+      <c r="C42" s="148"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="148"/>
+      <c r="F42" s="148"/>
+      <c r="G42" s="148"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="149"/>
-      <c r="C43" s="149"/>
-      <c r="D43" s="149"/>
-      <c r="E43" s="149"/>
-      <c r="F43" s="149"/>
-      <c r="G43" s="149"/>
+      <c r="B43" s="148"/>
+      <c r="C43" s="148"/>
+      <c r="D43" s="148"/>
+      <c r="E43" s="148"/>
+      <c r="F43" s="148"/>
+      <c r="G43" s="148"/>
     </row>
     <row r="44" spans="2:7" ht="25.95" customHeight="1">
-      <c r="B44" s="152"/>
-      <c r="C44" s="152"/>
-      <c r="D44" s="152"/>
-      <c r="E44" s="152"/>
-      <c r="F44" s="152"/>
-      <c r="G44" s="152"/>
+      <c r="B44" s="151"/>
+      <c r="C44" s="151"/>
+      <c r="D44" s="151"/>
+      <c r="E44" s="151"/>
+      <c r="F44" s="151"/>
+      <c r="G44" s="151"/>
     </row>
     <row r="45" spans="2:7">
       <c r="B45" s="99"/>
@@ -38932,8 +38942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EE127B-7B53-574B-9873-73BCF871E1D2}">
   <dimension ref="C3:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="143" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:H8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -38951,14 +38961,14 @@
       <c r="F3" s="103"/>
     </row>
     <row r="4" spans="3:8" ht="18">
-      <c r="C4" s="156" t="s">
+      <c r="C4" s="152" t="s">
         <v>306</v>
       </c>
-      <c r="D4" s="156"/>
-      <c r="E4" s="156"/>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
     </row>
     <row r="5" spans="3:8" ht="16.2" thickBot="1">
       <c r="C5" s="115" t="s">
@@ -39045,14 +39055,14 @@
     </row>
     <row r="10" spans="3:8" ht="12" customHeight="1"/>
     <row r="11" spans="3:8" ht="21" customHeight="1">
-      <c r="C11" s="156" t="s">
+      <c r="C11" s="152" t="s">
         <v>308</v>
       </c>
-      <c r="D11" s="156"/>
-      <c r="E11" s="156"/>
-      <c r="F11" s="156"/>
-      <c r="G11" s="156"/>
-      <c r="H11" s="156"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="152"/>
+      <c r="F11" s="152"/>
+      <c r="G11" s="152"/>
+      <c r="H11" s="152"/>
     </row>
     <row r="12" spans="3:8" ht="16.2" thickBot="1">
       <c r="C12" s="113" t="s">
@@ -39061,14 +39071,14 @@
       <c r="D12" s="114" t="s">
         <v>297</v>
       </c>
-      <c r="E12" s="153" t="s">
+      <c r="E12" s="154" t="s">
         <v>296</v>
       </c>
-      <c r="F12" s="153"/>
-      <c r="G12" s="153" t="s">
+      <c r="F12" s="154"/>
+      <c r="G12" s="154" t="s">
         <v>298</v>
       </c>
-      <c r="H12" s="153"/>
+      <c r="H12" s="154"/>
     </row>
     <row r="13" spans="3:8">
       <c r="C13" s="117" t="s">
@@ -39141,14 +39151,14 @@
       <c r="F17" s="108"/>
     </row>
     <row r="18" spans="3:8" ht="18">
-      <c r="C18" s="157" t="s">
+      <c r="C18" s="153" t="s">
         <v>305</v>
       </c>
-      <c r="D18" s="157"/>
-      <c r="E18" s="157"/>
-      <c r="F18" s="157"/>
-      <c r="G18" s="157"/>
-      <c r="H18" s="157"/>
+      <c r="D18" s="153"/>
+      <c r="E18" s="153"/>
+      <c r="F18" s="153"/>
+      <c r="G18" s="153"/>
+      <c r="H18" s="153"/>
     </row>
     <row r="19" spans="3:8" ht="19.2" thickBot="1">
       <c r="C19" s="113" t="s">
@@ -39157,14 +39167,14 @@
       <c r="D19" s="114" t="s">
         <v>302</v>
       </c>
-      <c r="E19" s="153" t="s">
+      <c r="E19" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="153"/>
-      <c r="G19" s="153" t="s">
+      <c r="F19" s="154"/>
+      <c r="G19" s="154" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="153"/>
+      <c r="H19" s="154"/>
     </row>
     <row r="20" spans="3:8">
       <c r="C20" s="108" t="s">
@@ -39173,17 +39183,25 @@
       <c r="D20" s="108">
         <v>2.0687000000000002</v>
       </c>
-      <c r="E20" s="154">
+      <c r="E20" s="156">
         <v>3</v>
       </c>
-      <c r="F20" s="154"/>
-      <c r="G20" s="154">
+      <c r="F20" s="156"/>
+      <c r="G20" s="156">
         <v>0.55830000000000002</v>
       </c>
-      <c r="H20" s="154"/>
+      <c r="H20" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="C18:H18"/>
     <mergeCell ref="C4:H4"/>
@@ -39193,14 +39211,6 @@
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>